<commit_message>
Updated ZAF model - 2025-08-01 02:10
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A7A3ECC-C1F2-4870-9439-8814029DFD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A50F967-CF17-47E7-A62E-44EF4E8372E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0916h11,Wb0121h09,RaD,Wb0122h11,Wb0122h15,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,TaD,Wb0122h12,Tc0917h08,Tc0917h17,Tc0916h10,Tc0917h14,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10</t>
-  </si>
-  <si>
-    <t>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,RaN,Tc0917h20,Wb0122h20,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h04,Tc0916h24,Tc0917h05,Tc0917h19,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,TaN,Tc0916h03,Tc0916h23,SaP,Tc0916h06,Tc0917h01</t>
+    <t>Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,Tc0916h10,Tc0917h14,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,TaD,Wb0122h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h08,Tc0917h17</t>
+  </si>
+  <si>
+    <t>Tc0916h04,SaP,Tc0916h06,Tc0917h01,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,RaN,Tc0917h20,Wb0122h20,Tc0917h23,Wb0121h02,Wb0121h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0917h23,Wb0121h02,Wb0121h06,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,RaN,Tc0917h20,Wb0122h20,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,Tc0916h04,Tc0916h24,Tc0917h05,Tc0917h19,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,TaN,Tc0916h03,Tc0916h23,SaP,Tc0916h06,Tc0917h01</v>
+        <v>Tc0916h04,SaP,Tc0916h06,Tc0917h01,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,RaN,Tc0917h20,Wb0122h20,Tc0917h23,Wb0121h02,Wb0121h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0916h11,Wb0121h09,RaD,Wb0122h11,Wb0122h15,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,TaD,Wb0122h12,Tc0917h08,Tc0917h17,Tc0916h10,Tc0917h14,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10</v>
+        <v>Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,Tc0916h10,Tc0917h14,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,TaD,Wb0122h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h08,Tc0917h17</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BA9974F-6715-46AE-BAAF-1797FEEE18D7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE8B689-15C7-4DB9-9C94-ED248F7A9027}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68CD66DC-8DDA-45F6-ABFA-9B14BFA39CB0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF96D01A-9128-484A-B579-A5D488020DDC}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3079,7 +3079,7 @@
         <v>29</v>
       </c>
       <c r="N4">
-        <v>0.14835493519441675</v>
+        <v>0.14835493519441678</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>0.17228315054835494</v>
+        <v>0.39361914257228325</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="N6">
-        <v>0.39361914257228325</v>
+        <v>0.17228315054835494</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9315249A-628B-4410-A1D0-BE7944357638}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDD9FE2-6ED9-4972-A044-0C7D08A28026}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-08-01 02:16
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A50F967-CF17-47E7-A62E-44EF4E8372E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C70C5F-E856-4CD2-A4A0-EED03AAC75BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,Tc0916h10,Tc0917h14,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,TaD,Wb0122h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h08,Tc0917h17</t>
-  </si>
-  <si>
-    <t>Tc0916h04,SaP,Tc0916h06,Tc0917h01,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,RaN,Tc0917h20,Wb0122h20,Tc0917h23,Wb0121h02,Wb0121h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02</t>
+    <t>Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h11,Wb0121h09,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0917h08,Tc0917h17,Tc0916h12,Wb0121h13,TaD,Wb0122h12,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Wb0121h14,Wb0121h16</t>
+  </si>
+  <si>
+    <t>Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaP,Tc0916h06,Tc0917h01,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,RaN,Tc0917h20,Wb0122h20,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,TaN,Tc0916h03,Tc0916h23,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h04,Tc0917h02,Tc0917h06,WaP,Wb0122h22</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>Tc0916h04,SaP,Tc0916h06,Tc0917h01,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,TaN,Tc0916h03,Tc0916h23,Tc0917h24,Wb0121h05,Wb0121h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,RaN,Tc0917h20,Wb0122h20,Tc0917h23,Wb0121h02,Wb0121h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02</v>
+        <v>Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaP,Tc0916h06,Tc0917h01,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,RaN,Tc0917h20,Wb0122h20,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,TaN,Tc0916h03,Tc0916h23,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h04,Tc0917h02,Tc0917h06,WaP,Wb0122h22</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h11,Wb0121h09,Tc0917h11,WaD,Wb0122h08,Wb0122h18,RaD,Wb0122h11,Wb0122h15,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Wb0121h13,Tc0916h12,Tc0917h18,Wb0121h08,Wb0121h18,Wb0121h14,Wb0121h16,Tc0916h10,Tc0917h14,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,TaD,Wb0122h12,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h08,Tc0917h17</v>
+        <v>Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h11,Wb0121h09,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0917h08,Tc0917h17,Tc0916h12,Wb0121h13,TaD,Wb0122h12,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Wb0121h14,Wb0121h16</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EDE8B689-15C7-4DB9-9C94-ED248F7A9027}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0F34B-F75A-48F5-949E-47A3FDF0A9D4}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF96D01A-9128-484A-B579-A5D488020DDC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C5B2D1-E581-4800-9907-F9D0469538A5}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3076,10 +3076,10 @@
         <v>180</v>
       </c>
       <c r="M4" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="N4">
-        <v>0.14835493519441678</v>
+        <v>0.48574277168494512</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="N5">
-        <v>0.39361914257228325</v>
+        <v>0.17228315054835491</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N6">
-        <v>0.17228315054835494</v>
+        <v>0.39361914257228309</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -3181,10 +3181,10 @@
         <v>180</v>
       </c>
       <c r="M7" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="N7">
-        <v>0.48574277168494528</v>
+        <v>0.14835493519441673</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,7 +5900,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BDD9FE2-6ED9-4972-A044-0C7D08A28026}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C9E3B5-9D47-4001-80AA-39734C802D64}">
   <dimension ref="B2:O211"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated ZAF model - 2025-08-01 02:34
</commit_message>
<xml_diff>
--- a/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_108.xlsx
+++ b/VerveStacks_ZAF/SuppXLS/scen_tsparameters_ts_108.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ZAF\SuppXLS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C70C5F-E856-4CD2-A4A0-EED03AAC75BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFB0674-7D38-4623-A6BA-6D6D7F302EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="4" activeTab="4" xr2:uid="{693B72C3-6B34-4E45-9416-347F2176C33F}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1909" uniqueCount="302">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1933" uniqueCount="302">
   <si>
     <t>UC_N</t>
   </si>
@@ -921,10 +921,10 @@
     <t>day_night</t>
   </si>
   <si>
-    <t>Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h11,Wb0121h09,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0917h08,Tc0917h17,Tc0916h12,Wb0121h13,TaD,Wb0122h12,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Wb0121h14,Wb0121h16</t>
-  </si>
-  <si>
-    <t>Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaP,Tc0916h06,Tc0917h01,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,RaN,Tc0917h20,Wb0122h20,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,TaN,Tc0916h03,Tc0916h23,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h04,Tc0917h02,Tc0917h06,WaP,Wb0122h22</t>
+    <t>Tc0917h08,Tc0917h17,Tc0916h12,Wb0121h14,Wb0121h16,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h10,Tc0917h14,Tc0916h11,Wb0121h09,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0917h18,Wb0121h08,Wb0121h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,RaD,Wb0122h11,Wb0122h15,TaD,Wb0122h12</t>
+  </si>
+  <si>
+    <t>SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h24,Tc0917h05,Tc0917h19,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,SaP,Tc0916h06,Tc0917h01,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0917h23,Wb0121h02,Wb0121h06,TaN,Tc0916h03,Tc0916h23,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Wb0121h05,Wb0121h24,Tc0916h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaN,Tc0917h20,Wb0122h20</t>
   </si>
   <si>
     <t>elc_buildings</t>
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G7" t="str">
         <f>C14</f>
-        <v>Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,SaP,Tc0916h06,Tc0917h01,Tc0917h23,Wb0121h02,Wb0121h06,Wb0121h05,Wb0121h24,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,RaN,Tc0917h20,Wb0122h20,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,TaN,Tc0916h03,Tc0916h23,Tc0916h24,Tc0917h05,Tc0917h19,Tc0916h04,Tc0917h02,Tc0917h06,WaP,Wb0122h22</v>
+        <v>SaN,Tc0917h03,WaN,Wb0121h19,Wb0121h22,Wb0122h02,Tc0917h24,Tc0917h02,Tc0917h06,WaP,Wb0122h22,Tc0916h24,Tc0917h05,Tc0917h19,RaP,Tc0916h19,Wb0121h01,Wb0122h19,Wb0122h21,SaP,Tc0916h06,Tc0917h01,Tc0916h05,Tc0917h22,Wb0122h01,Wb0122h05,Wb0122h06,TaP,Tc0916h21,Wb0121h20,Wb0122h04,Tc0917h23,Wb0121h02,Wb0121h06,TaN,Tc0916h03,Tc0916h23,Tc0916h01,Tc0916h20,Tc0917h21,Wb0121h03,Wb0121h04,Wb0122h23,Wb0122h24,Wb0121h05,Wb0121h24,Tc0916h04,Tc0916h02,Tc0916h22,Tc0917h04,Wb0121h21,Wb0121h23,Wb0122h03,RaN,Tc0917h20,Wb0122h20</v>
       </c>
       <c r="H7">
         <f>1+H8</f>
@@ -1527,7 +1527,7 @@
       </c>
       <c r="G8" t="str">
         <f>C13</f>
-        <v>Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0917h18,Wb0121h08,Wb0121h18,Tc0916h11,Wb0121h09,RaD,Wb0122h11,Wb0122h15,Tc0916h10,Tc0917h14,Tc0917h08,Tc0917h17,Tc0916h12,Wb0121h13,TaD,Wb0122h12,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,Wb0121h14,Wb0121h16</v>
+        <v>Tc0917h08,Tc0917h17,Tc0916h12,Wb0121h14,Wb0121h16,Tc0917h11,WaD,Wb0122h08,Wb0122h18,Wb0121h13,Tc0916h08,Tc0916h09,Tc0916h17,Tc0917h10,Wb0121h12,SaD,Tc0917h16,Wb0121h07,Wb0122h10,Tc0916h10,Tc0917h14,Tc0916h11,Wb0121h09,Tc0916h07,Tc0916h14,Tc0916h16,Tc0917h15,Wb0121h11,Wb0122h13,Tc0916h15,Tc0917h07,Tc0917h09,Wb0122h09,Wb0122h16,Wb0122h17,Tc0916h13,Tc0916h18,Tc0917h13,Wb0121h15,Wb0121h17,Tc0917h18,Wb0121h08,Wb0121h18,Tc0917h12,Wb0121h10,Wb0122h07,Wb0122h14,RaD,Wb0122h11,Wb0122h15,TaD,Wb0122h12</v>
       </c>
       <c r="H8">
         <f>-$H$1</f>
@@ -2140,7 +2140,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2C0F34B-F75A-48F5-949E-47A3FDF0A9D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2EDF3B3-A6F5-426B-A8EF-3A96F44EFBFB}">
   <dimension ref="B2:F102"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2997,7 +2997,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C5B2D1-E581-4800-9907-F9D0469538A5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C50864-16A9-496C-98B6-FE276E3584E5}">
   <dimension ref="B2:O111"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3076,10 +3076,10 @@
         <v>180</v>
       </c>
       <c r="M4" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="N4">
-        <v>0.48574277168494512</v>
+        <v>0.17228315054835494</v>
       </c>
       <c r="O4" t="s">
         <v>300</v>
@@ -3111,10 +3111,10 @@
         <v>180</v>
       </c>
       <c r="M5" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="N5">
-        <v>0.17228315054835491</v>
+        <v>0.3936191425722832</v>
       </c>
       <c r="O5" t="s">
         <v>300</v>
@@ -3146,10 +3146,10 @@
         <v>180</v>
       </c>
       <c r="M6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="N6">
-        <v>0.39361914257228309</v>
+        <v>0.48574277168494528</v>
       </c>
       <c r="O6" t="s">
         <v>300</v>
@@ -3184,7 +3184,7 @@
         <v>29</v>
       </c>
       <c r="N7">
-        <v>0.14835493519441673</v>
+        <v>0.14835493519441675</v>
       </c>
       <c r="O7" t="s">
         <v>300</v>
@@ -5900,8 +5900,8 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C9E3B5-9D47-4001-80AA-39734C802D64}">
-  <dimension ref="B2:O211"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13F32164-51AA-418A-8A26-76AC6BB6C332}">
+  <dimension ref="B2:O219"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5970,7 +5970,7 @@
         <v>178</v>
       </c>
       <c r="J4">
-        <v>0.15698113307482336</v>
+        <v>0.14911396696068191</v>
       </c>
       <c r="M4" t="s">
         <v>14</v>
@@ -5979,7 +5979,7 @@
         <v>178</v>
       </c>
       <c r="O4">
-        <v>0.13363419092319107</v>
+        <v>0.14767510779818793</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.45">
@@ -6002,7 +6002,7 @@
         <v>181</v>
       </c>
       <c r="J5">
-        <v>6.3800399400598298E-2</v>
+        <v>7.1401087970968211E-2</v>
       </c>
       <c r="M5" t="s">
         <v>14</v>
@@ -6011,7 +6011,7 @@
         <v>181</v>
       </c>
       <c r="O5">
-        <v>0.17004374800125466</v>
+        <v>0.22520499117390669</v>
       </c>
     </row>
     <row r="6" spans="2:15" x14ac:dyDescent="0.45">
@@ -6034,7 +6034,7 @@
         <v>182</v>
       </c>
       <c r="J6">
-        <v>2.416408338836783E-2</v>
+        <v>2.4465515157931779E-2</v>
       </c>
       <c r="M6" t="s">
         <v>14</v>
@@ -6043,7 +6043,7 @@
         <v>182</v>
       </c>
       <c r="O6">
-        <v>6.9415004962052107E-2</v>
+        <v>6.9473984339850636E-2</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.45">
@@ -6066,7 +6066,7 @@
         <v>183</v>
       </c>
       <c r="J7">
-        <v>0.17549524994275525</v>
+        <v>0.16631280563297862</v>
       </c>
       <c r="M7" t="s">
         <v>14</v>
@@ -6075,7 +6075,7 @@
         <v>183</v>
       </c>
       <c r="O7">
-        <v>0.16523765102001819</v>
+        <v>0.1819638741569336</v>
       </c>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.45">
@@ -6098,7 +6098,7 @@
         <v>184</v>
       </c>
       <c r="J8">
-        <v>6.9988989435793195E-2</v>
+        <v>7.7661223845831795E-2</v>
       </c>
       <c r="M8" t="s">
         <v>14</v>
@@ -6107,7 +6107,7 @@
         <v>184</v>
       </c>
       <c r="O8">
-        <v>0.1787354398365828</v>
+        <v>0.23430887064572503</v>
       </c>
     </row>
     <row r="9" spans="2:15" x14ac:dyDescent="0.45">
@@ -6130,7 +6130,7 @@
         <v>185</v>
       </c>
       <c r="J9">
-        <v>2.742697811404228E-2</v>
+        <v>2.8604248949723129E-2</v>
       </c>
       <c r="M9" t="s">
         <v>14</v>
@@ -6139,7 +6139,7 @@
         <v>185</v>
       </c>
       <c r="O9">
-        <v>9.3246527435216997E-2</v>
+        <v>0.10685979669547474</v>
       </c>
     </row>
     <row r="10" spans="2:15" x14ac:dyDescent="0.45">
@@ -6162,7 +6162,7 @@
         <v>186</v>
       </c>
       <c r="J10">
-        <v>0.15023271662690602</v>
+        <v>0.14248479647088114</v>
       </c>
       <c r="M10" t="s">
         <v>14</v>
@@ -6171,7 +6171,7 @@
         <v>186</v>
       </c>
       <c r="O10">
-        <v>0.13937816468974629</v>
+        <v>0.15429175440016363</v>
       </c>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.45">
@@ -6194,7 +6194,7 @@
         <v>187</v>
       </c>
       <c r="J11">
-        <v>6.0066814075893288E-2</v>
+        <v>6.7641149195623473E-2</v>
       </c>
       <c r="M11" t="s">
         <v>14</v>
@@ -6203,7 +6203,7 @@
         <v>187</v>
       </c>
       <c r="O11">
-        <v>0.1614476395684139</v>
+        <v>0.20456927426558202</v>
       </c>
     </row>
     <row r="12" spans="2:15" x14ac:dyDescent="0.45">
@@ -6226,7 +6226,7 @@
         <v>188</v>
       </c>
       <c r="J12">
-        <v>2.2888608999232854E-2</v>
+        <v>2.3139874840190908E-2</v>
       </c>
       <c r="M12" t="s">
         <v>14</v>
@@ -6235,7 +6235,7 @@
         <v>188</v>
       </c>
       <c r="O12">
-        <v>4.7685987075025915E-2</v>
+        <v>4.3040333224193761E-2</v>
       </c>
     </row>
     <row r="13" spans="2:15" x14ac:dyDescent="0.45">
@@ -6258,7 +6258,7 @@
         <v>189</v>
       </c>
       <c r="J13">
-        <v>7.1881595074280337E-5</v>
+        <v>7.1677785769211957E-5</v>
       </c>
       <c r="M13" t="s">
         <v>14</v>
@@ -6290,7 +6290,7 @@
         <v>190</v>
       </c>
       <c r="J14">
-        <v>7.1881595074280337E-5</v>
+        <v>6.9967605000686826E-5</v>
       </c>
       <c r="M14" t="s">
         <v>14</v>
@@ -6322,7 +6322,7 @@
         <v>191</v>
       </c>
       <c r="J15">
-        <v>7.3867990126430215E-5</v>
+        <v>6.9967605000686826E-5</v>
       </c>
       <c r="M15" t="s">
         <v>14</v>
@@ -6354,7 +6354,7 @@
         <v>192</v>
       </c>
       <c r="J16">
-        <v>8.6945594025994493E-5</v>
+        <v>7.1901108343796013E-5</v>
       </c>
       <c r="M16" t="s">
         <v>14</v>
@@ -6386,7 +6386,7 @@
         <v>193</v>
       </c>
       <c r="J17">
-        <v>9.7324357231604343E-5</v>
+        <v>8.463049509508626E-5</v>
       </c>
       <c r="M17" t="s">
         <v>14</v>
@@ -6418,7 +6418,7 @@
         <v>194</v>
       </c>
       <c r="J18">
-        <v>1.1877621625983699E-4</v>
+        <v>9.4732903140085287E-5</v>
       </c>
       <c r="M18" t="s">
         <v>14</v>
@@ -6450,7 +6450,7 @@
         <v>195</v>
       </c>
       <c r="J19">
-        <v>1.3397908173495368E-4</v>
+        <v>1.1561356386369301E-4</v>
       </c>
       <c r="M19" t="s">
         <v>14</v>
@@ -6482,7 +6482,7 @@
         <v>196</v>
       </c>
       <c r="J20">
-        <v>1.3921978357466825E-4</v>
+        <v>1.3041162288481437E-4</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -6514,7 +6514,7 @@
         <v>197</v>
       </c>
       <c r="J21">
-        <v>1.397873250181397E-4</v>
+        <v>1.3551278064110242E-4</v>
       </c>
       <c r="M21" t="s">
         <v>14</v>
@@ -6546,7 +6546,7 @@
         <v>198</v>
       </c>
       <c r="J22">
-        <v>1.4109146280313778E-4</v>
+        <v>1.3606521016770504E-4</v>
       </c>
       <c r="M22" t="s">
         <v>14</v>
@@ -6578,7 +6578,7 @@
         <v>199</v>
       </c>
       <c r="J23">
-        <v>1.4099486000424907E-4</v>
+        <v>1.3733462269691958E-4</v>
       </c>
       <c r="M23" t="s">
         <v>14</v>
@@ -6610,7 +6610,7 @@
         <v>200</v>
       </c>
       <c r="J24">
-        <v>1.4097070930452684E-4</v>
+        <v>1.3724059213919999E-4</v>
       </c>
       <c r="M24" t="s">
         <v>14</v>
@@ -6642,7 +6642,7 @@
         <v>201</v>
       </c>
       <c r="J25">
-        <v>1.405118460098053E-4</v>
+        <v>1.3721708449977005E-4</v>
       </c>
       <c r="M25" t="s">
         <v>14</v>
@@ -6674,7 +6674,7 @@
         <v>202</v>
       </c>
       <c r="J26">
-        <v>1.4017373621369466E-4</v>
+        <v>1.3677043935060199E-4</v>
       </c>
       <c r="M26" t="s">
         <v>14</v>
@@ -6706,7 +6706,7 @@
         <v>203</v>
       </c>
       <c r="J27">
-        <v>1.3877903330473837E-4</v>
+        <v>1.3644133239858341E-4</v>
       </c>
       <c r="M27" t="s">
         <v>14</v>
@@ -6738,7 +6738,7 @@
         <v>204</v>
       </c>
       <c r="J28">
-        <v>1.4099486000424905E-4</v>
+        <v>1.3508376622150674E-4</v>
       </c>
       <c r="M28" t="s">
         <v>14</v>
@@ -6770,7 +6770,7 @@
         <v>205</v>
       </c>
       <c r="J29">
-        <v>1.4099486000424907E-4</v>
+        <v>1.3724059213920001E-4</v>
       </c>
       <c r="M29" t="s">
         <v>14</v>
@@ -6802,7 +6802,7 @@
         <v>206</v>
       </c>
       <c r="J30">
-        <v>1.4217824429063619E-4</v>
+        <v>1.3724059213919999E-4</v>
       </c>
       <c r="M30" t="s">
         <v>14</v>
@@ -6834,7 +6834,7 @@
         <v>207</v>
       </c>
       <c r="J31">
-        <v>1.3903261565182136E-4</v>
+        <v>1.3839246647126503E-4</v>
       </c>
       <c r="M31" t="s">
         <v>14</v>
@@ -6866,7 +6866,7 @@
         <v>208</v>
       </c>
       <c r="J32">
-        <v>1.2975874695850156E-4</v>
+        <v>1.3533059643552068E-4</v>
       </c>
       <c r="M32" t="s">
         <v>14</v>
@@ -6898,7 +6898,7 @@
         <v>209</v>
       </c>
       <c r="J33">
-        <v>1.1852263391275404E-4</v>
+        <v>1.2630366289443951E-4</v>
       </c>
       <c r="M33" t="s">
         <v>14</v>
@@ -6930,7 +6930,7 @@
         <v>210</v>
       </c>
       <c r="J34">
-        <v>9.2711573584666648E-5</v>
+        <v>1.1536673364967906E-4</v>
       </c>
       <c r="M34" t="s">
         <v>14</v>
@@ -6962,7 +6962,7 @@
         <v>211</v>
       </c>
       <c r="J35">
-        <v>8.1849796384613022E-5</v>
+        <v>9.0242944008974622E-5</v>
       </c>
       <c r="M35" t="s">
         <v>14</v>
@@ -6991,16 +6991,16 @@
         <v>295</v>
       </c>
       <c r="I36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J36">
-        <v>7.188159507428035E-5</v>
+        <v>7.9670383175377591E-5</v>
       </c>
       <c r="M36" t="s">
         <v>14</v>
       </c>
       <c r="N36" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="O36">
         <v>0</v>
@@ -7023,16 +7023,16 @@
         <v>295</v>
       </c>
       <c r="I37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J37">
-        <v>7.188159507428035E-5</v>
+        <v>7.1677785769211984E-5</v>
       </c>
       <c r="M37" t="s">
         <v>14</v>
       </c>
       <c r="N37" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="O37">
         <v>0</v>
@@ -7055,16 +7055,16 @@
         <v>295</v>
       </c>
       <c r="I38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J38">
-        <v>7.3867990126430243E-5</v>
+        <v>6.996760500068684E-5</v>
       </c>
       <c r="M38" t="s">
         <v>14</v>
       </c>
       <c r="N38" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="O38">
         <v>0</v>
@@ -7087,16 +7087,16 @@
         <v>295</v>
       </c>
       <c r="I39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J39">
-        <v>8.694559402599452E-5</v>
+        <v>6.996760500068684E-5</v>
       </c>
       <c r="M39" t="s">
         <v>14</v>
       </c>
       <c r="N39" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="O39">
         <v>0</v>
@@ -7119,16 +7119,16 @@
         <v>295</v>
       </c>
       <c r="I40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J40">
-        <v>9.732435723160437E-5</v>
+        <v>7.1901108343796027E-5</v>
       </c>
       <c r="M40" t="s">
         <v>14</v>
       </c>
       <c r="N40" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="O40">
         <v>0</v>
@@ -7151,16 +7151,16 @@
         <v>295</v>
       </c>
       <c r="I41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J41">
-        <v>1.1877621625983699E-4</v>
+        <v>8.4630495095086288E-5</v>
       </c>
       <c r="M41" t="s">
         <v>14</v>
       </c>
       <c r="N41" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="O41">
         <v>0</v>
@@ -7183,16 +7183,16 @@
         <v>295</v>
       </c>
       <c r="I42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J42">
-        <v>1.3397908173495368E-4</v>
+        <v>9.4732903140085315E-5</v>
       </c>
       <c r="M42" t="s">
         <v>14</v>
       </c>
       <c r="N42" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="O42">
         <v>0</v>
@@ -7215,16 +7215,16 @@
         <v>295</v>
       </c>
       <c r="I43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J43">
-        <v>1.3921978357466828E-4</v>
+        <v>1.1561356386369301E-4</v>
       </c>
       <c r="M43" t="s">
         <v>14</v>
       </c>
       <c r="N43" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="O43">
         <v>0</v>
@@ -7247,16 +7247,16 @@
         <v>295</v>
       </c>
       <c r="I44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J44">
-        <v>1.4007109573987539E-4</v>
+        <v>1.3041162288481437E-4</v>
       </c>
       <c r="M44" t="s">
         <v>14</v>
       </c>
       <c r="N44" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O44">
         <v>0</v>
@@ -7279,16 +7279,16 @@
         <v>295</v>
       </c>
       <c r="I45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J45">
-        <v>1.4159862749730373E-4</v>
+        <v>1.3551278064110242E-4</v>
       </c>
       <c r="M45" t="s">
         <v>14</v>
       </c>
       <c r="N45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="O45">
         <v>0</v>
@@ -7311,16 +7311,16 @@
         <v>295</v>
       </c>
       <c r="I46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J46">
-        <v>1.4121825397667929E-4</v>
+        <v>1.3634142493100637E-4</v>
       </c>
       <c r="M46" t="s">
         <v>14</v>
       </c>
       <c r="N46" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="O46">
         <v>0</v>
@@ -7343,16 +7343,16 @@
         <v>295</v>
       </c>
       <c r="I47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J47">
-        <v>1.4030052738723615E-4</v>
+        <v>1.3782828312494747E-4</v>
       </c>
       <c r="M47" t="s">
         <v>14</v>
       </c>
       <c r="N47" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O47">
         <v>0</v>
@@ -7375,16 +7375,16 @@
         <v>295</v>
       </c>
       <c r="I48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J48">
-        <v>1.4074731533209666E-4</v>
+        <v>1.3745803780392657E-4</v>
       </c>
       <c r="M48" t="s">
         <v>14</v>
       </c>
       <c r="N48" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O48">
         <v>0</v>
@@ -7407,16 +7407,16 @@
         <v>295</v>
       </c>
       <c r="I49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J49">
-        <v>1.4074731533209666E-4</v>
+        <v>1.3656474750559043E-4</v>
       </c>
       <c r="M49" t="s">
         <v>14</v>
       </c>
       <c r="N49" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O49">
         <v>0</v>
@@ -7439,16 +7439,16 @@
         <v>295</v>
       </c>
       <c r="I50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J50">
-        <v>1.3921978357466831E-4</v>
+        <v>1.3699963883504355E-4</v>
       </c>
       <c r="M50" t="s">
         <v>14</v>
       </c>
       <c r="N50" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O50">
         <v>0</v>
@@ -7471,16 +7471,16 @@
         <v>295</v>
       </c>
       <c r="I51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J51">
-        <v>1.4099486000424907E-4</v>
+        <v>1.3699963883504355E-4</v>
       </c>
       <c r="M51" t="s">
         <v>14</v>
       </c>
       <c r="N51" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="O51">
         <v>0</v>
@@ -7503,16 +7503,16 @@
         <v>295</v>
       </c>
       <c r="I52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J52">
-        <v>1.4099486000424907E-4</v>
+        <v>1.3551278064110242E-4</v>
       </c>
       <c r="M52" t="s">
         <v>14</v>
       </c>
       <c r="N52" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O52">
         <v>0</v>
@@ -7535,16 +7535,16 @@
         <v>295</v>
       </c>
       <c r="I53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J53">
-        <v>1.4217824429063622E-4</v>
+        <v>1.3724059213920001E-4</v>
       </c>
       <c r="M53" t="s">
         <v>14</v>
       </c>
       <c r="N53" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="O53">
         <v>0</v>
@@ -7567,16 +7567,16 @@
         <v>295</v>
       </c>
       <c r="I54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="J54">
-        <v>1.3903261565182136E-4</v>
+        <v>1.3724059213920001E-4</v>
       </c>
       <c r="M54" t="s">
         <v>14</v>
       </c>
       <c r="N54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="O54">
         <v>0</v>
@@ -7599,16 +7599,16 @@
         <v>295</v>
       </c>
       <c r="I55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="J55">
-        <v>1.2975874695850156E-4</v>
+        <v>1.3839246647126506E-4</v>
       </c>
       <c r="M55" t="s">
         <v>14</v>
       </c>
       <c r="N55" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="O55">
         <v>0</v>
@@ -7631,16 +7631,16 @@
         <v>295</v>
       </c>
       <c r="I56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="J56">
-        <v>1.1852263391275404E-4</v>
+        <v>1.353305964355207E-4</v>
       </c>
       <c r="M56" t="s">
         <v>14</v>
       </c>
       <c r="N56" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="O56">
         <v>0</v>
@@ -7663,16 +7663,16 @@
         <v>295</v>
       </c>
       <c r="I57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="J57">
-        <v>9.2711573584666662E-5</v>
+        <v>1.2630366289443951E-4</v>
       </c>
       <c r="M57" t="s">
         <v>14</v>
       </c>
       <c r="N57" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="O57">
         <v>0</v>
@@ -7695,16 +7695,16 @@
         <v>295</v>
       </c>
       <c r="I58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="J58">
-        <v>8.1849796384613049E-5</v>
+        <v>1.1536673364967907E-4</v>
       </c>
       <c r="M58" t="s">
         <v>14</v>
       </c>
       <c r="N58" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="O58">
         <v>0</v>
@@ -7727,19 +7727,19 @@
         <v>295</v>
       </c>
       <c r="I59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J59">
-        <v>0.15299359278847693</v>
+        <v>9.0242944008974636E-5</v>
       </c>
       <c r="M59" t="s">
         <v>14</v>
       </c>
       <c r="N59" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="O59">
-        <v>0.15169955718528128</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="2:15" x14ac:dyDescent="0.45">
@@ -7759,19 +7759,19 @@
         <v>295</v>
       </c>
       <c r="I60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J60">
-        <v>6.2157537746890437E-2</v>
+        <v>7.9670383175377605E-5</v>
       </c>
       <c r="M60" t="s">
         <v>14</v>
       </c>
       <c r="N60" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="O60">
-        <v>0.15537768469394608</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="2:15" x14ac:dyDescent="0.45">
@@ -7791,19 +7791,19 @@
         <v>295</v>
       </c>
       <c r="I61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J61">
-        <v>2.2640971651549598E-2</v>
+        <v>0.14549629391367155</v>
       </c>
       <c r="M61" t="s">
         <v>14</v>
       </c>
       <c r="N61" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="O61">
-        <v>4.9807352721212395E-2</v>
+        <v>0.16541311857634367</v>
       </c>
     </row>
     <row r="62" spans="2:15" x14ac:dyDescent="0.45">
@@ -7823,19 +7823,19 @@
         <v>295</v>
       </c>
       <c r="I62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J62">
-        <v>7.5998792030174098E-5</v>
+        <v>6.9594560142280659E-2</v>
       </c>
       <c r="M62" t="s">
         <v>14</v>
       </c>
       <c r="N62" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="O62">
-        <v>0</v>
+        <v>0.18928899468198801</v>
       </c>
     </row>
     <row r="63" spans="2:15" x14ac:dyDescent="0.45">
@@ -7855,19 +7855,19 @@
         <v>295</v>
       </c>
       <c r="I63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J63">
-        <v>7.5998792030174098E-5</v>
+        <v>2.2926964095661206E-2</v>
       </c>
       <c r="M63" t="s">
         <v>14</v>
       </c>
       <c r="N63" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="O63">
-        <v>0</v>
+        <v>4.1464814849328624E-2</v>
       </c>
     </row>
     <row r="64" spans="2:15" x14ac:dyDescent="0.45">
@@ -7887,16 +7887,16 @@
         <v>295</v>
       </c>
       <c r="I64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J64">
-        <v>8.124553154481924E-5</v>
+        <v>7.4539356765906665E-5</v>
       </c>
       <c r="M64" t="s">
         <v>14</v>
       </c>
       <c r="N64" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O64">
         <v>0</v>
@@ -7919,16 +7919,16 @@
         <v>295</v>
       </c>
       <c r="I65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J65">
-        <v>9.0151102067375708E-5</v>
+        <v>7.3975173419589069E-5</v>
       </c>
       <c r="M65" t="s">
         <v>14</v>
       </c>
       <c r="N65" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="O65">
         <v>0</v>
@@ -7951,16 +7951,16 @@
         <v>295</v>
       </c>
       <c r="I66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J66">
-        <v>1.0075929692034636E-4</v>
+        <v>7.3975173419589069E-5</v>
       </c>
       <c r="M66" t="s">
         <v>14</v>
       </c>
       <c r="N66" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="O66">
         <v>0</v>
@@ -7983,16 +7983,16 @@
         <v>295</v>
       </c>
       <c r="I67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="J67">
-        <v>1.2034551439504003E-4</v>
+        <v>7.908220808573461E-5</v>
       </c>
       <c r="M67" t="s">
         <v>14</v>
       </c>
       <c r="N67" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="O67">
         <v>0</v>
@@ -8015,16 +8015,16 @@
         <v>295</v>
       </c>
       <c r="I68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J68">
-        <v>1.3491442400244936E-4</v>
+        <v>8.7750650125509828E-5</v>
       </c>
       <c r="M68" t="s">
         <v>14</v>
       </c>
       <c r="N68" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="O68">
         <v>0</v>
@@ -8047,16 +8047,16 @@
         <v>295</v>
       </c>
       <c r="I69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J69">
-        <v>1.3844646383681921E-4</v>
+        <v>9.8076380745092925E-5</v>
       </c>
       <c r="M69" t="s">
         <v>14</v>
       </c>
       <c r="N69" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="O69">
         <v>0</v>
@@ -8079,16 +8079,16 @@
         <v>295</v>
       </c>
       <c r="I70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="J70">
-        <v>1.4427885781972738E-4</v>
+        <v>1.1714107632274093E-4</v>
       </c>
       <c r="M70" t="s">
         <v>14</v>
       </c>
       <c r="N70" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="O70">
         <v>0</v>
@@ -8111,16 +8111,16 @@
         <v>295</v>
       </c>
       <c r="I71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="J71">
-        <v>1.4671807849166824E-4</v>
+        <v>1.3132205980882747E-4</v>
       </c>
       <c r="M71" t="s">
         <v>14</v>
       </c>
       <c r="N71" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="O71">
         <v>0</v>
@@ -8143,16 +8143,16 @@
         <v>295</v>
       </c>
       <c r="I72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="J72">
-        <v>1.4662147569277951E-4</v>
+        <v>1.3476005207545014E-4</v>
       </c>
       <c r="M72" t="s">
         <v>14</v>
       </c>
       <c r="N72" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="O72">
         <v>0</v>
@@ -8175,16 +8175,16 @@
         <v>295</v>
       </c>
       <c r="I73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="J73">
-        <v>1.4662147569277951E-4</v>
+        <v>1.4043714699777074E-4</v>
       </c>
       <c r="M73" t="s">
         <v>14</v>
       </c>
       <c r="N73" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="O73">
         <v>0</v>
@@ -8207,16 +8207,16 @@
         <v>295</v>
       </c>
       <c r="I74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="J74">
-        <v>1.449430020620875E-4</v>
+        <v>1.4281141858019054E-4</v>
       </c>
       <c r="M74" t="s">
         <v>14</v>
       </c>
       <c r="N74" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="O74">
         <v>0</v>
@@ -8239,16 +8239,16 @@
         <v>295</v>
       </c>
       <c r="I75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="J75">
-        <v>1.4325245308153441E-4</v>
+        <v>1.4271738802247092E-4</v>
       </c>
       <c r="M75" t="s">
         <v>14</v>
       </c>
       <c r="N75" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="O75">
         <v>0</v>
@@ -8271,16 +8271,16 @@
         <v>295</v>
       </c>
       <c r="I76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="J76">
-        <v>1.3786080936855618E-4</v>
+        <v>1.4271738802247095E-4</v>
       </c>
       <c r="M76" t="s">
         <v>14</v>
       </c>
       <c r="N76" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="O76">
         <v>0</v>
@@ -8303,16 +8303,16 @@
         <v>295</v>
       </c>
       <c r="I77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="J77">
-        <v>1.4007663606806683E-4</v>
+        <v>1.4108360708209295E-4</v>
       </c>
       <c r="M77" t="s">
         <v>14</v>
       </c>
       <c r="N77" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="O77">
         <v>0</v>
@@ -8335,16 +8335,16 @@
         <v>295</v>
       </c>
       <c r="I78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="J78">
-        <v>1.4043285888896907E-4</v>
+        <v>1.3943807232200003E-4</v>
       </c>
       <c r="M78" t="s">
         <v>14</v>
       </c>
       <c r="N78" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="O78">
         <v>0</v>
@@ -8367,16 +8367,16 @@
         <v>295</v>
       </c>
       <c r="I79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="J79">
-        <v>1.4161624317535627E-4</v>
+        <v>1.3418999181927512E-4</v>
       </c>
       <c r="M79" t="s">
         <v>14</v>
       </c>
       <c r="N79" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="O79">
         <v>0</v>
@@ -8399,16 +8399,16 @@
         <v>295</v>
       </c>
       <c r="I80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="J80">
-        <v>1.3781250796911183E-4</v>
+        <v>1.3634681773696831E-4</v>
       </c>
       <c r="M80" t="s">
         <v>14</v>
       </c>
       <c r="N80" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="O80">
         <v>0</v>
@@ -8431,16 +8431,16 @@
         <v>295</v>
       </c>
       <c r="I81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="J81">
-        <v>1.2672733679662798E-4</v>
+        <v>1.3669355541855933E-4</v>
       </c>
       <c r="M81" t="s">
         <v>14</v>
       </c>
       <c r="N81" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="O81">
         <v>0</v>
@@ -8463,16 +8463,16 @@
         <v>295</v>
       </c>
       <c r="I82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="J82">
-        <v>1.1780969092421039E-4</v>
+        <v>1.378454297506244E-4</v>
       </c>
       <c r="M82" t="s">
         <v>14</v>
       </c>
       <c r="N82" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="O82">
         <v>0</v>
@@ -8495,16 +8495,16 @@
         <v>295</v>
       </c>
       <c r="I83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="J83">
-        <v>9.5198598309312798E-5</v>
+        <v>1.3414297654041528E-4</v>
       </c>
       <c r="M83" t="s">
         <v>14</v>
       </c>
       <c r="N83" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="O83">
         <v>0</v>
@@ -8527,16 +8527,16 @@
         <v>295</v>
       </c>
       <c r="I84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="J84">
-        <v>8.361230011759359E-5</v>
+        <v>1.2335297004209173E-4</v>
       </c>
       <c r="M84" t="s">
         <v>14</v>
       </c>
       <c r="N84" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="O84">
         <v>0</v>
@@ -8559,16 +8559,16 @@
         <v>295</v>
       </c>
       <c r="I85" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="J85">
-        <v>7.3994283953232587E-5</v>
+        <v>1.1467277418260155E-4</v>
       </c>
       <c r="M85" t="s">
         <v>14</v>
       </c>
       <c r="N85" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="O85">
         <v>0</v>
@@ -8591,16 +8591,16 @@
         <v>295</v>
       </c>
       <c r="I86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="J86">
-        <v>7.3318064361011344E-5</v>
+        <v>9.2663746766358701E-5</v>
       </c>
       <c r="M86" t="s">
         <v>14</v>
       </c>
       <c r="N86" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="O86">
         <v>0</v>
@@ -8623,16 +8623,16 @@
         <v>295</v>
       </c>
       <c r="I87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="J87">
-        <v>7.8806310872878333E-5</v>
+        <v>8.1385956749864725E-5</v>
       </c>
       <c r="M87" t="s">
         <v>14</v>
       </c>
       <c r="N87" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="O87">
         <v>0</v>
@@ -8655,16 +8655,16 @@
         <v>295</v>
       </c>
       <c r="I88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="J88">
-        <v>8.7717919070365373E-5</v>
+        <v>7.3928158140729286E-5</v>
       </c>
       <c r="M88" t="s">
         <v>14</v>
       </c>
       <c r="N88" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="O88">
         <v>0</v>
@@ -8687,16 +8687,16 @@
         <v>295</v>
       </c>
       <c r="I89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="J89">
-        <v>1.0008911500305567E-4</v>
+        <v>7.2024039346907473E-5</v>
       </c>
       <c r="M89" t="s">
         <v>14</v>
       </c>
       <c r="N89" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="O89">
         <v>0</v>
@@ -8719,16 +8719,16 @@
         <v>295</v>
       </c>
       <c r="I90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="J90">
-        <v>1.2037570276969279E-4</v>
+        <v>7.1365825442870298E-5</v>
       </c>
       <c r="M90" t="s">
         <v>14</v>
       </c>
       <c r="N90" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="O90">
         <v>0</v>
@@ -8751,16 +8751,16 @@
         <v>295</v>
       </c>
       <c r="I91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="J91">
-        <v>1.3491442400244931E-4</v>
+        <v>7.6707936503314807E-5</v>
       </c>
       <c r="M91" t="s">
         <v>14</v>
       </c>
       <c r="N91" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="O91">
         <v>0</v>
@@ -8783,16 +8783,16 @@
         <v>295</v>
       </c>
       <c r="I92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="J92">
-        <v>1.3886910108195749E-4</v>
+        <v>8.5382255452947536E-5</v>
       </c>
       <c r="M92" t="s">
         <v>14</v>
       </c>
       <c r="N92" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="O92">
         <v>0</v>
@@ -8815,16 +8815,16 @@
         <v>295</v>
       </c>
       <c r="I93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="J93">
-        <v>1.4450828946708814E-4</v>
+        <v>9.7424043750913233E-5</v>
       </c>
       <c r="M93" t="s">
         <v>14</v>
       </c>
       <c r="N93" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="O93">
         <v>0</v>
@@ -8847,16 +8847,16 @@
         <v>295</v>
       </c>
       <c r="I94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="J94">
-        <v>1.5379423351026905E-4</v>
+        <v>1.1717046087202829E-4</v>
       </c>
       <c r="M94" t="s">
         <v>14</v>
       </c>
       <c r="N94" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="O94">
         <v>0</v>
@@ -8879,16 +8879,16 @@
         <v>295</v>
       </c>
       <c r="I95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="J95">
-        <v>1.5085992349402332E-4</v>
+        <v>1.3132205980882742E-4</v>
       </c>
       <c r="M95" t="s">
         <v>14</v>
       </c>
       <c r="N95" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="O95">
         <v>0</v>
@@ -8911,16 +8911,16 @@
         <v>295</v>
       </c>
       <c r="I96" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="J96">
-        <v>1.5085992349402332E-4</v>
+        <v>1.3517143576547336E-4</v>
       </c>
       <c r="M96" t="s">
         <v>14</v>
       </c>
       <c r="N96" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="O96">
         <v>0</v>
@@ -8943,16 +8943,16 @@
         <v>295</v>
       </c>
       <c r="I97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="J97">
-        <v>1.4918144986333134E-4</v>
+        <v>1.4066046957235477E-4</v>
       </c>
       <c r="M97" t="s">
         <v>14</v>
       </c>
       <c r="N97" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="O97">
         <v>0</v>
@@ -8975,16 +8975,16 @@
         <v>295</v>
       </c>
       <c r="I98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="J98">
-        <v>1.4589091702618337E-4</v>
+        <v>1.4969915693315087E-4</v>
       </c>
       <c r="M98" t="s">
         <v>14</v>
       </c>
       <c r="N98" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="O98">
         <v>0</v>
@@ -9007,16 +9007,16 @@
         <v>295</v>
       </c>
       <c r="I99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="J99">
-        <v>1.3838608708751374E-4</v>
+        <v>1.4684297874241817E-4</v>
       </c>
       <c r="M99" t="s">
         <v>14</v>
       </c>
       <c r="N99" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="O99">
         <v>0</v>
@@ -9039,16 +9039,16 @@
         <v>295</v>
       </c>
       <c r="I100" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="J100">
-        <v>1.4060191378702439E-4</v>
+        <v>1.4684297874241817E-4</v>
       </c>
       <c r="M100" t="s">
         <v>14</v>
       </c>
       <c r="N100" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="O100">
         <v>0</v>
@@ -9071,16 +9071,16 @@
         <v>295</v>
       </c>
       <c r="I101" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="J101">
-        <v>1.4043285888896907E-4</v>
+        <v>1.4520919780204022E-4</v>
       </c>
       <c r="M101" t="s">
         <v>14</v>
       </c>
       <c r="N101" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="O101">
         <v>0</v>
@@ -9103,16 +9103,16 @@
         <v>295</v>
       </c>
       <c r="I102" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J102">
-        <v>1.4161624317535627E-4</v>
+        <v>1.4200628192971652E-4</v>
       </c>
       <c r="M102" t="s">
         <v>14</v>
       </c>
       <c r="N102" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="O102">
         <v>0</v>
@@ -9135,16 +9135,16 @@
         <v>295</v>
       </c>
       <c r="I103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="J103">
-        <v>1.3781250796911183E-4</v>
+        <v>1.3470128297687539E-4</v>
       </c>
       <c r="M103" t="s">
         <v>14</v>
       </c>
       <c r="N103" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="O103">
         <v>0</v>
@@ -9167,16 +9167,16 @@
         <v>295</v>
       </c>
       <c r="I104" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="J104">
-        <v>1.2699903216850257E-4</v>
+        <v>1.3685810889456867E-4</v>
       </c>
       <c r="M104" t="s">
         <v>14</v>
       </c>
       <c r="N104" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="O104">
         <v>0</v>
@@ -9199,16 +9199,16 @@
         <v>295</v>
       </c>
       <c r="I105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="J105">
-        <v>1.1780969092421039E-4</v>
+        <v>1.3669355541855933E-4</v>
       </c>
       <c r="M105" t="s">
         <v>14</v>
       </c>
       <c r="N105" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="O105">
         <v>0</v>
@@ -9231,16 +9231,16 @@
         <v>295</v>
       </c>
       <c r="I106" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="J106">
-        <v>9.4981242011813114E-5</v>
+        <v>1.378454297506244E-4</v>
       </c>
       <c r="M106" t="s">
         <v>14</v>
       </c>
       <c r="N106" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="O106">
         <v>0</v>
@@ -9263,16 +9263,16 @@
         <v>295</v>
       </c>
       <c r="I107" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="J107">
-        <v>8.3612300117593563E-5</v>
+        <v>1.3414297654041528E-4</v>
       </c>
       <c r="M107" t="s">
         <v>14</v>
       </c>
       <c r="N107" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="O107">
         <v>0</v>
@@ -9292,13 +9292,22 @@
         <v>291</v>
       </c>
       <c r="H108" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I108" t="s">
-        <v>178</v>
+        <v>284</v>
       </c>
       <c r="J108">
-        <v>0.1433449377564199</v>
+        <v>1.2361743098567805E-4</v>
+      </c>
+      <c r="M108" t="s">
+        <v>14</v>
+      </c>
+      <c r="N108" t="s">
+        <v>284</v>
+      </c>
+      <c r="O108">
+        <v>0</v>
       </c>
     </row>
     <row r="109" spans="2:15" x14ac:dyDescent="0.45">
@@ -9315,13 +9324,22 @@
         <v>291</v>
       </c>
       <c r="H109" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I109" t="s">
-        <v>181</v>
+        <v>285</v>
       </c>
       <c r="J109">
-        <v>8.6616938881018096E-2</v>
+        <v>1.1467277418260155E-4</v>
+      </c>
+      <c r="M109" t="s">
+        <v>14</v>
+      </c>
+      <c r="N109" t="s">
+        <v>285</v>
+      </c>
+      <c r="O109">
+        <v>0</v>
       </c>
     </row>
     <row r="110" spans="2:15" x14ac:dyDescent="0.45">
@@ -9338,13 +9356,22 @@
         <v>291</v>
       </c>
       <c r="H110" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I110" t="s">
-        <v>182</v>
+        <v>286</v>
       </c>
       <c r="J110">
-        <v>2.2053706378496806E-2</v>
+        <v>9.2452178011489611E-5</v>
+      </c>
+      <c r="M110" t="s">
+        <v>14</v>
+      </c>
+      <c r="N110" t="s">
+        <v>286</v>
+      </c>
+      <c r="O110">
+        <v>0</v>
       </c>
     </row>
     <row r="111" spans="2:15" x14ac:dyDescent="0.45">
@@ -9361,13 +9388,22 @@
         <v>291</v>
       </c>
       <c r="H111" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="I111" t="s">
-        <v>183</v>
+        <v>287</v>
       </c>
       <c r="J111">
-        <v>0.14356943657598828</v>
+        <v>8.1385956749864698E-5</v>
+      </c>
+      <c r="M111" t="s">
+        <v>14</v>
+      </c>
+      <c r="N111" t="s">
+        <v>287</v>
+      </c>
+      <c r="O111">
+        <v>0</v>
       </c>
     </row>
     <row r="112" spans="2:15" x14ac:dyDescent="0.45">
@@ -9375,10 +9411,10 @@
         <v>296</v>
       </c>
       <c r="I112" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="J112">
-        <v>8.6501970578679976E-2</v>
+        <v>0.13729885231683758</v>
       </c>
     </row>
     <row r="113" spans="8:10" x14ac:dyDescent="0.45">
@@ -9386,10 +9422,10 @@
         <v>296</v>
       </c>
       <c r="I113" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="J113">
-        <v>2.2108406445529302E-2</v>
+        <v>9.3527751962487499E-2</v>
       </c>
     </row>
     <row r="114" spans="8:10" x14ac:dyDescent="0.45">
@@ -9397,10 +9433,10 @@
         <v>296</v>
       </c>
       <c r="I114" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="J114">
-        <v>0.13867576211693525</v>
+        <v>2.1195970279540996E-2</v>
       </c>
     </row>
     <row r="115" spans="8:10" x14ac:dyDescent="0.45">
@@ -9408,10 +9444,10 @@
         <v>296</v>
       </c>
       <c r="I115" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="J115">
-        <v>8.3763991229191023E-2</v>
+        <v>0.13747475593990818</v>
       </c>
     </row>
     <row r="116" spans="8:10" x14ac:dyDescent="0.45">
@@ -9419,10 +9455,10 @@
         <v>296</v>
       </c>
       <c r="I116" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="J116">
-        <v>2.1323833141833608E-2</v>
+        <v>9.337895204285053E-2</v>
       </c>
     </row>
     <row r="117" spans="8:10" x14ac:dyDescent="0.45">
@@ -9430,10 +9466,10 @@
         <v>296</v>
       </c>
       <c r="I117" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="J117">
-        <v>1.1704624193942443E-4</v>
+        <v>2.1294561924603311E-2</v>
       </c>
     </row>
     <row r="118" spans="8:10" x14ac:dyDescent="0.45">
@@ -9441,10 +9477,10 @@
         <v>296</v>
       </c>
       <c r="I118" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="J118">
-        <v>1.1704624193942443E-4</v>
+        <v>0.13281796440406418</v>
       </c>
     </row>
     <row r="119" spans="8:10" x14ac:dyDescent="0.45">
@@ -9452,10 +9488,10 @@
         <v>296</v>
       </c>
       <c r="I119" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="J119">
-        <v>1.1714284653105948E-4</v>
+        <v>9.0465345893233656E-2</v>
       </c>
     </row>
     <row r="120" spans="8:10" x14ac:dyDescent="0.45">
@@ -9463,10 +9499,10 @@
         <v>296</v>
       </c>
       <c r="I120" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="J120">
-        <v>1.1777885122857169E-4</v>
+        <v>2.0491951214251649E-2</v>
       </c>
     </row>
     <row r="121" spans="8:10" x14ac:dyDescent="0.45">
@@ -9474,10 +9510,10 @@
         <v>296</v>
       </c>
       <c r="I121" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="J121">
-        <v>1.1828360287909037E-4</v>
+        <v>1.1233561446239411E-4</v>
       </c>
     </row>
     <row r="122" spans="8:10" x14ac:dyDescent="0.45">
@@ -9485,10 +9521,10 @@
         <v>296</v>
       </c>
       <c r="I122" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="J122">
-        <v>1.1932687374255334E-4</v>
+        <v>1.1225366654496469E-4</v>
       </c>
     </row>
     <row r="123" spans="8:10" x14ac:dyDescent="0.45">
@@ -9496,10 +9532,10 @@
         <v>296</v>
       </c>
       <c r="I123" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="J123">
-        <v>1.2006623654418571E-4</v>
+        <v>1.1225366654496469E-4</v>
       </c>
     </row>
     <row r="124" spans="8:10" x14ac:dyDescent="0.45">
@@ -9507,10 +9543,10 @@
         <v>296</v>
       </c>
       <c r="I124" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="J124">
-        <v>1.2032110823275479E-4</v>
+        <v>1.1234631556501375E-4</v>
       </c>
     </row>
     <row r="125" spans="8:10" x14ac:dyDescent="0.45">
@@ -9518,10 +9554,10 @@
         <v>296</v>
       </c>
       <c r="I125" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="J125">
-        <v>1.203487095446505E-4</v>
+        <v>1.1295627841433372E-4</v>
       </c>
     </row>
     <row r="126" spans="8:10" x14ac:dyDescent="0.45">
@@ -9529,10 +9565,10 @@
         <v>296</v>
       </c>
       <c r="I126" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="J126">
-        <v>1.2041213383581516E-4</v>
+        <v>1.1344036250389097E-4</v>
       </c>
     </row>
     <row r="127" spans="8:10" x14ac:dyDescent="0.45">
@@ -9540,10 +9576,10 @@
         <v>296</v>
       </c>
       <c r="I127" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="J127">
-        <v>1.2040743574017333E-4</v>
+        <v>1.144409155988281E-4</v>
       </c>
     </row>
     <row r="128" spans="8:10" x14ac:dyDescent="0.45">
@@ -9551,10 +9587,10 @@
         <v>296</v>
       </c>
       <c r="I128" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="J128">
-        <v>1.2040626121626288E-4</v>
+        <v>1.1515000445136165E-4</v>
       </c>
     </row>
     <row r="129" spans="8:10" x14ac:dyDescent="0.45">
@@ -9562,10 +9598,10 @@
         <v>296</v>
       </c>
       <c r="I129" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="J129">
-        <v>1.203839452619642E-4</v>
+        <v>1.1539444016383153E-4</v>
       </c>
     </row>
     <row r="130" spans="8:10" x14ac:dyDescent="0.45">
@@ -9573,10 +9609,10 @@
         <v>296</v>
       </c>
       <c r="I130" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="J130">
-        <v>1.2036750192721781E-4</v>
+        <v>1.1542091131241697E-4</v>
       </c>
     </row>
     <row r="131" spans="8:10" x14ac:dyDescent="0.45">
@@ -9584,10 +9620,10 @@
         <v>296</v>
       </c>
       <c r="I131" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="J131">
-        <v>1.2029967317138896E-4</v>
+        <v>1.1548173863257076E-4</v>
       </c>
     </row>
     <row r="132" spans="8:10" x14ac:dyDescent="0.45">
@@ -9595,10 +9631,10 @@
         <v>296</v>
       </c>
       <c r="I132" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="J132">
-        <v>1.2040743574017333E-4</v>
+        <v>1.1547723290515196E-4</v>
       </c>
     </row>
     <row r="133" spans="8:10" x14ac:dyDescent="0.45">
@@ -9606,10 +9642,10 @@
         <v>296</v>
       </c>
       <c r="I133" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="J133">
-        <v>1.2040743574017333E-4</v>
+        <v>1.1547610647329726E-4</v>
       </c>
     </row>
     <row r="134" spans="8:10" x14ac:dyDescent="0.45">
@@ -9617,10 +9653,10 @@
         <v>296</v>
       </c>
       <c r="I134" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="J134">
-        <v>1.2046498741178571E-4</v>
+        <v>1.1545470426805797E-4</v>
       </c>
     </row>
     <row r="135" spans="8:10" x14ac:dyDescent="0.45">
@@ -9628,10 +9664,10 @@
         <v>296</v>
       </c>
       <c r="I135" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="J135">
-        <v>1.2031200567244875E-4</v>
+        <v>1.1543893422209217E-4</v>
       </c>
     </row>
     <row r="136" spans="8:10" x14ac:dyDescent="0.45">
@@ -9639,10 +9675,10 @@
         <v>296</v>
       </c>
       <c r="I136" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="J136">
-        <v>1.1986098849083345E-4</v>
+        <v>1.1537388278248326E-4</v>
       </c>
     </row>
     <row r="137" spans="8:10" x14ac:dyDescent="0.45">
@@ -9650,10 +9686,10 @@
         <v>296</v>
       </c>
       <c r="I137" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="J137">
-        <v>1.1931454124149356E-4</v>
+        <v>1.1547723290515196E-4</v>
       </c>
     </row>
     <row r="138" spans="8:10" x14ac:dyDescent="0.45">
@@ -9661,10 +9697,10 @@
         <v>296</v>
       </c>
       <c r="I138" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="J138">
-        <v>1.1805926881219316E-4</v>
+        <v>1.1547723290515196E-4</v>
       </c>
     </row>
     <row r="139" spans="8:10" x14ac:dyDescent="0.45">
@@ -9672,10 +9708,10 @@
         <v>296</v>
       </c>
       <c r="I139" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="J139">
-        <v>1.1753102668346536E-4</v>
+        <v>1.1553242806603226E-4</v>
       </c>
     </row>
     <row r="140" spans="8:10" x14ac:dyDescent="0.45">
@@ -9683,10 +9719,10 @@
         <v>296</v>
       </c>
       <c r="I140" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="J140">
-        <v>1.1704624193942442E-4</v>
+        <v>1.153857103169576E-4</v>
       </c>
     </row>
     <row r="141" spans="8:10" x14ac:dyDescent="0.45">
@@ -9694,10 +9730,10 @@
         <v>296</v>
       </c>
       <c r="I141" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="J141">
-        <v>1.1704624193942442E-4</v>
+        <v>1.1495316048475286E-4</v>
       </c>
     </row>
     <row r="142" spans="8:10" x14ac:dyDescent="0.45">
@@ -9705,10 +9741,10 @@
         <v>296</v>
       </c>
       <c r="I142" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="J142">
-        <v>1.1714284653105945E-4</v>
+        <v>1.1442908806435377E-4</v>
       </c>
     </row>
     <row r="143" spans="8:10" x14ac:dyDescent="0.45">
@@ -9716,10 +9752,10 @@
         <v>296</v>
       </c>
       <c r="I143" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="J143">
-        <v>1.1777885122857166E-4</v>
+        <v>1.1322521401964329E-4</v>
       </c>
     </row>
     <row r="144" spans="8:10" x14ac:dyDescent="0.45">
@@ -9727,10 +9763,10 @@
         <v>296</v>
       </c>
       <c r="I144" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="J144">
-        <v>1.1828360287909035E-4</v>
+        <v>1.1271860129299204E-4</v>
       </c>
     </row>
     <row r="145" spans="8:10" x14ac:dyDescent="0.45">
@@ -9738,10 +9774,10 @@
         <v>296</v>
       </c>
       <c r="I145" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="J145">
-        <v>1.1932687374255334E-4</v>
+        <v>1.1233561446239408E-4</v>
       </c>
     </row>
     <row r="146" spans="8:10" x14ac:dyDescent="0.45">
@@ -9749,10 +9785,10 @@
         <v>296</v>
       </c>
       <c r="I146" t="s">
-        <v>219</v>
+        <v>214</v>
       </c>
       <c r="J146">
-        <v>1.2006623654418571E-4</v>
+        <v>1.1225366654496467E-4</v>
       </c>
     </row>
     <row r="147" spans="8:10" x14ac:dyDescent="0.45">
@@ -9760,10 +9796,10 @@
         <v>296</v>
       </c>
       <c r="I147" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="J147">
-        <v>1.2032110823275476E-4</v>
+        <v>1.1225366654496467E-4</v>
       </c>
     </row>
     <row r="148" spans="8:10" x14ac:dyDescent="0.45">
@@ -9771,10 +9807,10 @@
         <v>296</v>
       </c>
       <c r="I148" t="s">
-        <v>221</v>
+        <v>216</v>
       </c>
       <c r="J148">
-        <v>1.2036251020059835E-4</v>
+        <v>1.1234631556501373E-4</v>
       </c>
     </row>
     <row r="149" spans="8:10" x14ac:dyDescent="0.45">
@@ -9782,10 +9818,10 @@
         <v>296</v>
       </c>
       <c r="I149" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="J149">
-        <v>1.2043679883793474E-4</v>
+        <v>1.129562784143337E-4</v>
       </c>
     </row>
     <row r="150" spans="8:10" x14ac:dyDescent="0.45">
@@ -9793,10 +9829,10 @@
         <v>296</v>
       </c>
       <c r="I150" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="J150">
-        <v>1.2041830008634504E-4</v>
+        <v>1.1344036250389096E-4</v>
       </c>
     </row>
     <row r="151" spans="8:10" x14ac:dyDescent="0.45">
@@ -9804,10 +9840,10 @@
         <v>296</v>
       </c>
       <c r="I151" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="J151">
-        <v>1.203736681777477E-4</v>
+        <v>1.144409155988281E-4</v>
       </c>
     </row>
     <row r="152" spans="8:10" x14ac:dyDescent="0.45">
@@ -9815,10 +9851,10 @@
         <v>296</v>
       </c>
       <c r="I152" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="J152">
-        <v>1.2039539687009114E-4</v>
+        <v>1.1515000445136165E-4</v>
       </c>
     </row>
     <row r="153" spans="8:10" x14ac:dyDescent="0.45">
@@ -9826,10 +9862,10 @@
         <v>296</v>
       </c>
       <c r="I153" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="J153">
-        <v>1.2039539687009114E-4</v>
+        <v>1.1539444016383152E-4</v>
       </c>
     </row>
     <row r="154" spans="8:10" x14ac:dyDescent="0.45">
@@ -9837,10 +9873,10 @@
         <v>296</v>
       </c>
       <c r="I154" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="J154">
-        <v>1.2032110823275476E-4</v>
+        <v>1.1543414688670967E-4</v>
       </c>
     </row>
     <row r="155" spans="8:10" x14ac:dyDescent="0.45">
@@ -9848,10 +9884,10 @@
         <v>296</v>
       </c>
       <c r="I155" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="J155">
-        <v>1.2040743574017331E-4</v>
+        <v>1.1550539370151945E-4</v>
       </c>
     </row>
     <row r="156" spans="8:10" x14ac:dyDescent="0.45">
@@ -9859,10 +9895,10 @@
         <v>296</v>
       </c>
       <c r="I156" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="J156">
-        <v>1.2040743574017331E-4</v>
+        <v>1.1548765239980792E-4</v>
       </c>
     </row>
     <row r="157" spans="8:10" x14ac:dyDescent="0.45">
@@ -9870,10 +9906,10 @@
         <v>296</v>
       </c>
       <c r="I157" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="J157">
-        <v>1.2046498741178569E-4</v>
+        <v>1.1544484798932934E-4</v>
       </c>
     </row>
     <row r="158" spans="8:10" x14ac:dyDescent="0.45">
@@ -9881,10 +9917,10 @@
         <v>296</v>
       </c>
       <c r="I158" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="J158">
-        <v>1.2031200567244873E-4</v>
+        <v>1.1546568697864127E-4</v>
       </c>
     </row>
     <row r="159" spans="8:10" x14ac:dyDescent="0.45">
@@ -9892,10 +9928,10 @@
         <v>296</v>
       </c>
       <c r="I159" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="J159">
-        <v>1.1986098849083342E-4</v>
+        <v>1.1546568697864127E-4</v>
       </c>
     </row>
     <row r="160" spans="8:10" x14ac:dyDescent="0.45">
@@ -9903,10 +9939,10 @@
         <v>296</v>
       </c>
       <c r="I160" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="J160">
-        <v>1.1931454124149355E-4</v>
+        <v>1.1539444016383152E-4</v>
       </c>
     </row>
     <row r="161" spans="8:10" x14ac:dyDescent="0.45">
@@ -9914,10 +9950,10 @@
         <v>296</v>
       </c>
       <c r="I161" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="J161">
-        <v>1.1805926881219316E-4</v>
+        <v>1.1547723290515194E-4</v>
       </c>
     </row>
     <row r="162" spans="8:10" x14ac:dyDescent="0.45">
@@ -9925,10 +9961,10 @@
         <v>296</v>
       </c>
       <c r="I162" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="J162">
-        <v>1.1753102668346533E-4</v>
+        <v>1.1547723290515194E-4</v>
       </c>
     </row>
     <row r="163" spans="8:10" x14ac:dyDescent="0.45">
@@ -9936,10 +9972,10 @@
         <v>296</v>
       </c>
       <c r="I163" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="J163">
-        <v>0.13715570565395938</v>
+        <v>1.1553242806603224E-4</v>
       </c>
     </row>
     <row r="164" spans="8:10" x14ac:dyDescent="0.45">
@@ -9947,10 +9983,10 @@
         <v>296</v>
       </c>
       <c r="I164" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="J164">
-        <v>8.2847622577426325E-2</v>
+        <v>1.1538571031695759E-4</v>
       </c>
     </row>
     <row r="165" spans="8:10" x14ac:dyDescent="0.45">
@@ -9958,10 +9994,10 @@
         <v>296</v>
       </c>
       <c r="I165" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="J165">
-        <v>2.1057277997205793E-2</v>
+        <v>1.1495316048475284E-4</v>
       </c>
     </row>
     <row r="166" spans="8:10" x14ac:dyDescent="0.45">
@@ -9969,10 +10005,10 @@
         <v>296</v>
       </c>
       <c r="I166" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J166">
-        <v>1.1704831228645575E-4</v>
+        <v>1.1442908806435374E-4</v>
       </c>
     </row>
     <row r="167" spans="8:10" x14ac:dyDescent="0.45">
@@ -9980,10 +10016,10 @@
         <v>296</v>
       </c>
       <c r="I167" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="J167">
-        <v>1.1704831228645575E-4</v>
+        <v>1.1322521401964329E-4</v>
       </c>
     </row>
     <row r="168" spans="8:10" x14ac:dyDescent="0.45">
@@ -9991,10 +10027,10 @@
         <v>296</v>
       </c>
       <c r="I168" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="J168">
-        <v>1.1730347760600242E-4</v>
+        <v>1.1271860129299203E-4</v>
       </c>
     </row>
     <row r="169" spans="8:10" x14ac:dyDescent="0.45">
@@ -10002,10 +10038,10 @@
         <v>296</v>
       </c>
       <c r="I169" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="J169">
-        <v>1.1773658329798325E-4</v>
+        <v>0.13137567997828634</v>
       </c>
     </row>
     <row r="170" spans="8:10" x14ac:dyDescent="0.45">
@@ -10013,10 +10049,10 @@
         <v>296</v>
       </c>
       <c r="I170" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="J170">
-        <v>1.1825249292565127E-4</v>
+        <v>8.9460541460678847E-2</v>
       </c>
     </row>
     <row r="171" spans="8:10" x14ac:dyDescent="0.45">
@@ -10024,10 +10060,10 @@
         <v>296</v>
       </c>
       <c r="I171" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="J171">
-        <v>1.1920503181703149E-4</v>
+        <v>2.0237658493834128E-2</v>
       </c>
     </row>
     <row r="172" spans="8:10" x14ac:dyDescent="0.45">
@@ -10035,10 +10071,10 @@
         <v>296</v>
       </c>
       <c r="I172" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="J172">
-        <v>1.1991356336601438E-4</v>
+        <v>1.1228268648407974E-4</v>
       </c>
     </row>
     <row r="173" spans="8:10" x14ac:dyDescent="0.45">
@@ -10046,10 +10082,10 @@
         <v>296</v>
       </c>
       <c r="I173" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="J173">
-        <v>1.2008533748791865E-4</v>
+        <v>1.1225565211956695E-4</v>
       </c>
     </row>
     <row r="174" spans="8:10" x14ac:dyDescent="0.45">
@@ -10057,10 +10093,10 @@
         <v>296</v>
       </c>
       <c r="I174" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="J174">
-        <v>1.2036898501229388E-4</v>
+        <v>1.1225565211956695E-4</v>
       </c>
     </row>
     <row r="175" spans="8:10" x14ac:dyDescent="0.45">
@@ -10068,10 +10104,10 @@
         <v>296</v>
       </c>
       <c r="I175" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="J175">
-        <v>1.2048761192724999E-4</v>
+        <v>1.1250036944000049E-4</v>
       </c>
     </row>
     <row r="176" spans="8:10" x14ac:dyDescent="0.45">
@@ -10079,10 +10115,10 @@
         <v>296</v>
       </c>
       <c r="I176" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="J176">
-        <v>1.2048291383160818E-4</v>
+        <v>1.1291574118642106E-4</v>
       </c>
     </row>
     <row r="177" spans="8:10" x14ac:dyDescent="0.45">
@@ -10090,10 +10126,10 @@
         <v>296</v>
       </c>
       <c r="I177" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="J177">
-        <v>1.2048291383160818E-4</v>
+        <v>1.1341052637859796E-4</v>
       </c>
     </row>
     <row r="178" spans="8:10" x14ac:dyDescent="0.45">
@@ -10101,10 +10137,10 @@
         <v>296</v>
       </c>
       <c r="I178" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="J178">
-        <v>1.2040128441983145E-4</v>
+        <v>1.1432406261275953E-4</v>
       </c>
     </row>
     <row r="179" spans="8:10" x14ac:dyDescent="0.45">
@@ -10112,10 +10148,10 @@
         <v>296</v>
       </c>
       <c r="I179" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="J179">
-        <v>1.203190677460995E-4</v>
+        <v>1.150035826291072E-4</v>
       </c>
     </row>
     <row r="180" spans="8:10" x14ac:dyDescent="0.45">
@@ -10123,10 +10159,10 @@
         <v>296</v>
       </c>
       <c r="I180" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="J180">
-        <v>1.2005685528309007E-4</v>
+        <v>1.1516832328785706E-4</v>
       </c>
     </row>
     <row r="181" spans="8:10" x14ac:dyDescent="0.45">
@@ -10134,10 +10170,10 @@
         <v>296</v>
       </c>
       <c r="I181" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="J181">
-        <v>1.2016461785187446E-4</v>
+        <v>1.1544035658076708E-4</v>
       </c>
     </row>
     <row r="182" spans="8:10" x14ac:dyDescent="0.45">
@@ -10145,10 +10181,10 @@
         <v>296</v>
       </c>
       <c r="I182" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="J182">
-        <v>1.201819420795537E-4</v>
+        <v>1.1555412619809176E-4</v>
       </c>
     </row>
     <row r="183" spans="8:10" x14ac:dyDescent="0.45">
@@ -10156,10 +10192,10 @@
         <v>296</v>
       </c>
       <c r="I183" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="J183">
-        <v>1.2023949375116605E-4</v>
+        <v>1.1554962047067297E-4</v>
       </c>
     </row>
     <row r="184" spans="8:10" x14ac:dyDescent="0.45">
@@ -10167,10 +10203,10 @@
         <v>296</v>
       </c>
       <c r="I184" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="J184">
-        <v>1.2005450623526916E-4</v>
+        <v>1.1554962047067297E-4</v>
       </c>
     </row>
     <row r="185" spans="8:10" x14ac:dyDescent="0.45">
@@ -10178,10 +10214,10 @@
         <v>296</v>
       </c>
       <c r="I185" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="J185">
-        <v>1.1951539976036962E-4</v>
+        <v>1.1547133345677133E-4</v>
       </c>
     </row>
     <row r="186" spans="8:10" x14ac:dyDescent="0.45">
@@ -10189,10 +10225,10 @@
         <v>296</v>
       </c>
       <c r="I186" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="J186">
-        <v>1.1908170680643357E-4</v>
+        <v>1.1539248322694234E-4</v>
       </c>
     </row>
     <row r="187" spans="8:10" x14ac:dyDescent="0.45">
@@ -10200,10 +10236,10 @@
         <v>296</v>
       </c>
       <c r="I187" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="J187">
-        <v>1.1798205879526866E-4</v>
+        <v>1.1514100731538059E-4</v>
       </c>
     </row>
     <row r="188" spans="8:10" x14ac:dyDescent="0.45">
@@ -10211,10 +10247,10 @@
         <v>296</v>
       </c>
       <c r="I188" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="J188">
-        <v>1.1741858094922714E-4</v>
+        <v>1.1524435743804932E-4</v>
       </c>
     </row>
     <row r="189" spans="8:10" x14ac:dyDescent="0.45">
@@ -10222,10 +10258,10 @@
         <v>296</v>
       </c>
       <c r="I189" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="J189">
-        <v>1.1695082680188786E-4</v>
+        <v>1.1526097230790612E-4</v>
       </c>
     </row>
     <row r="190" spans="8:10" x14ac:dyDescent="0.45">
@@ -10233,10 +10269,10 @@
         <v>296</v>
       </c>
       <c r="I190" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="J190">
-        <v>1.1691794013239506E-4</v>
+        <v>1.1531616746878642E-4</v>
       </c>
     </row>
     <row r="191" spans="8:10" x14ac:dyDescent="0.45">
@@ -10244,10 +10280,10 @@
         <v>296</v>
       </c>
       <c r="I191" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="J191">
-        <v>1.1718485069104631E-4</v>
+        <v>1.1513875445167119E-4</v>
       </c>
     </row>
     <row r="192" spans="8:10" x14ac:dyDescent="0.45">
@@ -10255,10 +10291,10 @@
         <v>296</v>
       </c>
       <c r="I192" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="J192">
-        <v>1.1761825001400475E-4</v>
+        <v>1.1462172223036396E-4</v>
       </c>
     </row>
     <row r="193" spans="8:10" x14ac:dyDescent="0.45">
@@ -10266,10 +10302,10 @@
         <v>296</v>
       </c>
       <c r="I193" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="J193">
-        <v>1.1821989988713611E-4</v>
+        <v>1.1420578726801605E-4</v>
       </c>
     </row>
     <row r="194" spans="8:10" x14ac:dyDescent="0.45">
@@ -10277,10 +10313,10 @@
         <v>296</v>
       </c>
       <c r="I194" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="J194">
-        <v>1.1920649997191956E-4</v>
+        <v>1.1315116544405332E-4</v>
       </c>
     </row>
     <row r="195" spans="8:10" x14ac:dyDescent="0.45">
@@ -10288,10 +10324,10 @@
         <v>296</v>
       </c>
       <c r="I195" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="J195">
-        <v>1.1991356336601439E-4</v>
+        <v>1.1261075976176107E-4</v>
       </c>
     </row>
     <row r="196" spans="8:10" x14ac:dyDescent="0.45">
@@ -10299,10 +10335,10 @@
         <v>296</v>
       </c>
       <c r="I196" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="J196">
-        <v>1.2010589165635163E-4</v>
+        <v>1.1225339925585755E-4</v>
       </c>
     </row>
     <row r="197" spans="8:10" x14ac:dyDescent="0.45">
@@ -10310,10 +10346,10 @@
         <v>296</v>
       </c>
       <c r="I197" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="J197">
-        <v>1.2038014298944324E-4</v>
+        <v>1.1216215827562686E-4</v>
       </c>
     </row>
     <row r="198" spans="8:10" x14ac:dyDescent="0.45">
@@ -10321,10 +10357,10 @@
         <v>296</v>
       </c>
       <c r="I198" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="J198">
-        <v>1.2083174743301377E-4</v>
+        <v>1.1213061818369526E-4</v>
       </c>
     </row>
     <row r="199" spans="8:10" x14ac:dyDescent="0.45">
@@ -10332,10 +10368,10 @@
         <v>296</v>
       </c>
       <c r="I199" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="J199">
-        <v>1.206890427778933E-4</v>
+        <v>1.1238659982267581E-4</v>
       </c>
     </row>
     <row r="200" spans="8:10" x14ac:dyDescent="0.45">
@@ -10343,10 +10379,10 @@
         <v>296</v>
       </c>
       <c r="I200" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="J200">
-        <v>1.206890427778933E-4</v>
+        <v>1.1280225317706004E-4</v>
       </c>
     </row>
     <row r="201" spans="8:10" x14ac:dyDescent="0.45">
@@ -10354,10 +10390,10 @@
         <v>296</v>
       </c>
       <c r="I201" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="J201">
-        <v>1.2060741336611656E-4</v>
+        <v>1.1337926789463004E-4</v>
       </c>
     </row>
     <row r="202" spans="8:10" x14ac:dyDescent="0.45">
@@ -10365,10 +10401,10 @@
         <v>296</v>
       </c>
       <c r="I202" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="J202">
-        <v>1.2044738448331686E-4</v>
+        <v>1.1432547065257791E-4</v>
       </c>
     </row>
     <row r="203" spans="8:10" x14ac:dyDescent="0.45">
@@ -10376,10 +10412,10 @@
         <v>296</v>
       </c>
       <c r="I203" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="J203">
-        <v>1.2008240117814251E-4</v>
+        <v>1.1500358262910723E-4</v>
       </c>
     </row>
     <row r="204" spans="8:10" x14ac:dyDescent="0.45">
@@ -10387,10 +10423,10 @@
         <v>296</v>
       </c>
       <c r="I204" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="J204">
-        <v>1.2019016374692689E-4</v>
+        <v>1.1518803584531432E-4</v>
       </c>
     </row>
     <row r="205" spans="8:10" x14ac:dyDescent="0.45">
@@ -10398,10 +10434,10 @@
         <v>296</v>
       </c>
       <c r="I205" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="J205">
-        <v>1.201819420795537E-4</v>
+        <v>1.1545105768338673E-4</v>
       </c>
     </row>
     <row r="206" spans="8:10" x14ac:dyDescent="0.45">
@@ -10409,10 +10445,10 @@
         <v>296</v>
       </c>
       <c r="I206" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="J206">
-        <v>1.2023949375116605E-4</v>
+        <v>1.1588417073151882E-4</v>
       </c>
     </row>
     <row r="207" spans="8:10" x14ac:dyDescent="0.45">
@@ -10420,10 +10456,10 @@
         <v>296</v>
       </c>
       <c r="I207" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="J207">
-        <v>1.2005450623526916E-4</v>
+        <v>1.1574730926117278E-4</v>
       </c>
     </row>
     <row r="208" spans="8:10" x14ac:dyDescent="0.45">
@@ -10431,10 +10467,10 @@
         <v>296</v>
       </c>
       <c r="I208" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="J208">
-        <v>1.1952861315436227E-4</v>
+        <v>1.1574730926117278E-4</v>
       </c>
     </row>
     <row r="209" spans="8:10" x14ac:dyDescent="0.45">
@@ -10442,10 +10478,10 @@
         <v>296</v>
       </c>
       <c r="I209" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="J209">
-        <v>1.1908170680643357E-4</v>
+        <v>1.1566902224727114E-4</v>
       </c>
     </row>
     <row r="210" spans="8:10" x14ac:dyDescent="0.45">
@@ -10453,10 +10489,10 @@
         <v>296</v>
       </c>
       <c r="I210" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="J210">
-        <v>1.1797148808007455E-4</v>
+        <v>1.1551554590706828E-4</v>
       </c>
     </row>
     <row r="211" spans="8:10" x14ac:dyDescent="0.45">
@@ -10464,10 +10500,98 @@
         <v>296</v>
       </c>
       <c r="I211" t="s">
+        <v>279</v>
+      </c>
+      <c r="J211">
+        <v>1.1516550720822032E-4</v>
+      </c>
+    </row>
+    <row r="212" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H212" t="s">
+        <v>296</v>
+      </c>
+      <c r="I212" t="s">
+        <v>280</v>
+      </c>
+      <c r="J212">
+        <v>1.1526885733088903E-4</v>
+      </c>
+    </row>
+    <row r="213" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H213" t="s">
+        <v>296</v>
+      </c>
+      <c r="I213" t="s">
+        <v>281</v>
+      </c>
+      <c r="J213">
+        <v>1.1526097230790612E-4</v>
+      </c>
+    </row>
+    <row r="214" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H214" t="s">
+        <v>296</v>
+      </c>
+      <c r="I214" t="s">
+        <v>282</v>
+      </c>
+      <c r="J214">
+        <v>1.1531616746878642E-4</v>
+      </c>
+    </row>
+    <row r="215" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H215" t="s">
+        <v>296</v>
+      </c>
+      <c r="I215" t="s">
+        <v>283</v>
+      </c>
+      <c r="J215">
+        <v>1.1513875445167119E-4</v>
+      </c>
+    </row>
+    <row r="216" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H216" t="s">
+        <v>296</v>
+      </c>
+      <c r="I216" t="s">
+        <v>284</v>
+      </c>
+      <c r="J216">
+        <v>1.1463439458872934E-4</v>
+      </c>
+    </row>
+    <row r="217" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H217" t="s">
+        <v>296</v>
+      </c>
+      <c r="I217" t="s">
+        <v>285</v>
+      </c>
+      <c r="J217">
+        <v>1.1420578726801605E-4</v>
+      </c>
+    </row>
+    <row r="218" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H218" t="s">
+        <v>296</v>
+      </c>
+      <c r="I218" t="s">
         <v>286</v>
       </c>
-      <c r="J211">
-        <v>1.1741858094922717E-4</v>
+      <c r="J218">
+        <v>1.1314102755736102E-4</v>
+      </c>
+    </row>
+    <row r="219" spans="8:10" x14ac:dyDescent="0.45">
+      <c r="H219" t="s">
+        <v>296</v>
+      </c>
+      <c r="I219" t="s">
+        <v>287</v>
+      </c>
+      <c r="J219">
+        <v>1.1261075976176108E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>